<commit_message>
Basic functions are complete
</commit_message>
<xml_diff>
--- a/DVF_Dogrobber/Lite DVF Configuration File_v0.2.xlsx
+++ b/DVF_Dogrobber/Lite DVF Configuration File_v0.2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="4" r:id="rId1"/>
@@ -195,16 +195,16 @@
     <t>Y</t>
   </si>
   <si>
+    <t>RGB LED</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>RGB LED function check</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>RGB LED</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>RGB LED function check</t>
   </si>
   <si>
     <r>
@@ -1916,8 +1916,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="13.8" outlineLevelCol="4"/>
@@ -1977,24 +1977,24 @@
         <v>27</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" s="32" customFormat="1" spans="1:5">
       <c r="A5" s="41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="C5" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="D5" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="42" t="s">
-        <v>28</v>
-      </c>
       <c r="E5" s="43" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2090,8 +2090,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="$A8:$XFD8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="13.8" outlineLevelCol="6"/>
@@ -2133,7 +2133,7 @@
       </c>
       <c r="G2" s="10" t="str">
         <f>'Global Configuration'!E4</f>
-        <v>N</v>
+        <v>Y</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -2252,7 +2252,7 @@
         <v>50</v>
       </c>
       <c r="C9" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>27</v>
@@ -2269,7 +2269,7 @@
         <v>52</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="16"/>
@@ -2284,7 +2284,7 @@
         <v>25</v>
       </c>
       <c r="C11" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="16"/>
@@ -2296,10 +2296,10 @@
         <v>54</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="16"/>
@@ -2314,7 +2314,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="28" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="16"/>

</xml_diff>